<commit_message>
raw pair angles service integration done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>rawOutagesCreationServiceUrl</t>
+  </si>
+  <si>
+    <t>rawPairAnglesCreationServiceUrl</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,9 +458,18 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
create raw voltage ui done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>rawPairAnglesCreationServiceUrl</t>
+  </si>
+  <si>
+    <t>rawFrequencyCreationServiceUrl</t>
+  </si>
+  <si>
+    <t>rawVoltageCreationServiceUrl</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,10 +472,28 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
derived volt creation ui done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>rawVoltageCreationServiceUrl</t>
+  </si>
+  <si>
+    <t>derivedVoltageCreationServiceUrl</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,12 +491,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
     <hyperlink ref="B5" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
derived weekly vdi creation UI done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>derivedVoltageCreationServiceUrl</t>
+  </si>
+  <si>
+    <t>derivedVdiCreationServiceUrl</t>
+  </si>
+  <si>
+    <t>derivedFrequencyCreationServiceUrl</t>
   </si>
 </sst>
 </file>
@@ -431,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -493,9 +499,25 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -506,6 +528,8 @@
     <hyperlink ref="B5" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4"/>
     <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dev or prod mode config with waitress setup done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>derivedFrequencyCreationServiceUrl</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -437,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,6 +525,14 @@
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
violation messages upload ui done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>iegcViolMsgsCreationServiceUrl</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -473,15 +476,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -489,7 +492,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -497,7 +500,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -505,7 +508,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -513,7 +516,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -521,7 +524,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -529,21 +532,30 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
-    <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="B10" r:id="rId7"/>
+    <hyperlink ref="B11" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
weekly report generation done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>lowVoltageNodeCreationServiceUrl</t>
+  </si>
+  <si>
+    <t>weeklyRepCreationServiceUrl</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,6 +593,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
@@ -601,6 +612,7 @@
     <hyperlink ref="B10" r:id="rId7"/>
     <hyperlink ref="B11" r:id="rId8"/>
     <hyperlink ref="B12:B15" r:id="rId9" display="http://google.com"/>
+    <hyperlink ref="B16" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reports listing page donw
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>weeklyRepCreationServiceUrl</t>
+  </si>
+  <si>
+    <t>path\to\folder</t>
+  </si>
+  <si>
+    <t>weeklyReportsFolderPath</t>
   </si>
 </sst>
 </file>
@@ -461,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,6 +605,14 @@
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -615,6 +629,7 @@
     <hyperlink ref="B16" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
display iegc viol msgs done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>derivedFrequencyFetchUrl</t>
+  </si>
+  <si>
+    <t>iegcViolMsgsFetchUrl</t>
   </si>
 </sst>
 </file>
@@ -470,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,6 +626,14 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -639,9 +650,10 @@
     <hyperlink ref="B12:B15" r:id="rId9" display="http://google.com"/>
     <hyperlink ref="B16" r:id="rId10"/>
     <hyperlink ref="B18" r:id="rId11"/>
+    <hyperlink ref="B19" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
trans and major Gen Outages fetch done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>iegcViolMsgsFetchUrl</t>
+  </si>
+  <si>
+    <t>transOutagesFetchUrl</t>
+  </si>
+  <si>
+    <t>majorGenOutagesFetchUrl</t>
+  </si>
+  <si>
+    <t>longUnrevForcedOutagesFetchUrl</t>
   </si>
 </sst>
 </file>
@@ -473,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,6 +643,30 @@
         <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -651,9 +684,11 @@
     <hyperlink ref="B16" r:id="rId10"/>
     <hyperlink ref="B18" r:id="rId11"/>
     <hyperlink ref="B19" r:id="rId12"/>
+    <hyperlink ref="B20" r:id="rId13"/>
+    <hyperlink ref="B21:B22" r:id="rId14" display="http://google.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
view raw outages done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>longUnrevForcedOutagesFetchUrl</t>
+  </si>
+  <si>
+    <t>outagesFetchUrl</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +651,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>3</v>
@@ -656,7 +659,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>3</v>
@@ -664,9 +667,17 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -684,11 +695,12 @@
     <hyperlink ref="B16" r:id="rId10"/>
     <hyperlink ref="B18" r:id="rId11"/>
     <hyperlink ref="B19" r:id="rId12"/>
-    <hyperlink ref="B20" r:id="rId13"/>
-    <hyperlink ref="B21:B22" r:id="rId14" display="http://google.com"/>
+    <hyperlink ref="B21" r:id="rId13"/>
+    <hyperlink ref="B22:B23" r:id="rId14" display="http://google.com"/>
+    <hyperlink ref="B20" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>